<commit_message>
added overview page sample training plan
</commit_message>
<xml_diff>
--- a/TrainingPlan.xlsx
+++ b/TrainingPlan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Rider" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="RampTest" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="build_1_2_VO2Max" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="build_1_3_endurance" sheetId="4" state="visible" r:id="rId5"/>
@@ -33,9 +33,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="52">
   <si>
     <t xml:space="preserve">FTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuesday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wednesday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thursday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Friday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saturday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build Phase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VO2Max 4x4min @ 106%
+4 min break</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endurance 1,5h @ 65-75%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endurance 2h @ 65%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SS 4x12min @ 95%
+5 min break</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endurance 2.5h @ 65%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group Ride</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target Watts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VO2Max 4x6min @ 106%
+5 min break</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SS 4x15min @ 90%
+5 min break</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VO2Max 4x8min @ 106%
+6 min break</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SS 3x20min @ 90%
+5 min break</t>
   </si>
   <si>
     <t xml:space="preserve">FILE NAME</t>
@@ -120,11 +201,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00\ %"/>
+    <numFmt numFmtId="165" formatCode="hh:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="0.00\ %"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -145,6 +227,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -194,7 +283,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -203,15 +292,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -232,74 +333,320 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:B16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="4" style="0" width="22.79"/>
+  </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>299</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>299</v>
+      <c r="B4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>1.0625</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>3.0625</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <f aca="false">SUM(D4:I4)</f>
+        <v>4.52083333333333</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
+      <c r="B5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">$B$1*1.06</f>
+        <v>316.94</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">$B$1*0.7</f>
+        <v>209.3</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <f aca="false">$B$1*0.65</f>
+        <v>194.35</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">$B$1*0.95</f>
+        <v>284.05</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">$B$1*0.65</f>
+        <v>194.35</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">$B$1*0.5</f>
+        <v>149.5</v>
+      </c>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
+      <c r="B7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="I7" s="4" t="n">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <f aca="false">SUM(D7:I7)</f>
+        <v>0.583333333333333</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
+      <c r="B8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">$B$1*1.06</f>
+        <v>316.94</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <f aca="false">$B$1*0.65</f>
+        <v>194.35</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <f aca="false">$B$1*0.65</f>
+        <v>194.35</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">$B$1*0.9</f>
+        <v>269.1</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">$B$1*0.65</f>
+        <v>194.35</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <f aca="false">$B$1*0.5</f>
+        <v>149.5</v>
+      </c>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
+      <c r="B10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="I10" s="4" t="n">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="J10" s="4" t="n">
+        <f aca="false">SUM(D10:I10)</f>
+        <v>0.604166666666667</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="2"/>
+      <c r="B11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">$B$1*1.06</f>
+        <v>316.94</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <f aca="false">$B$1*0.65</f>
+        <v>194.35</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <f aca="false">$B$1*0.65</f>
+        <v>194.35</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <f aca="false">$B$1*0.9</f>
+        <v>269.1</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <f aca="false">$B$1*0.65</f>
+        <v>194.35</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <f aca="false">$B$1*0.5</f>
+        <v>149.5</v>
+      </c>
+      <c r="J11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
+      <c r="B12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
+      <c r="B13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
+      <c r="B14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="3"/>
+      <c r="B15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="3"/>
+      <c r="B16" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -330,39 +677,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="n">
-        <f aca="false">Rider!B4</f>
+        <f aca="false">Overview!B1</f>
         <v>299</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -370,7 +717,7 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -378,7 +725,7 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="5" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -386,7 +733,7 @@
       <c r="A8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="5" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -394,7 +741,7 @@
       <c r="A9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -402,7 +749,7 @@
       <c r="A10" s="1" t="n">
         <v>115</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -410,7 +757,7 @@
       <c r="A11" s="0" t="n">
         <v>115</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -418,7 +765,7 @@
       <c r="A12" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -451,39 +798,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="n">
-        <f aca="false">Rider!B4</f>
+        <f aca="false">Overview!B1</f>
         <v>299</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -491,7 +838,7 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -499,7 +846,7 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="5" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -507,7 +854,7 @@
       <c r="A8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="5" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -515,7 +862,7 @@
       <c r="A9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -523,7 +870,7 @@
       <c r="A10" s="1" t="n">
         <v>115</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -531,7 +878,7 @@
       <c r="A11" s="0" t="n">
         <v>115</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -539,7 +886,7 @@
       <c r="A12" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -572,39 +919,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="n">
-        <f aca="false">Rider!B4</f>
+        <f aca="false">Overview!B1</f>
         <v>299</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -612,7 +959,7 @@
       <c r="A6" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -620,7 +967,7 @@
       <c r="A7" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="5" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -628,7 +975,7 @@
       <c r="A8" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="5" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -636,7 +983,7 @@
       <c r="A9" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -644,7 +991,7 @@
       <c r="A10" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -652,7 +999,7 @@
       <c r="A11" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -660,7 +1007,7 @@
       <c r="A12" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -668,7 +1015,7 @@
       <c r="A13" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="6" t="n">
         <v>0.93</v>
       </c>
     </row>
@@ -676,7 +1023,7 @@
       <c r="A14" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="6" t="n">
         <v>0.93</v>
       </c>
     </row>
@@ -684,7 +1031,7 @@
       <c r="A15" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -692,7 +1039,7 @@
       <c r="A16" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -700,7 +1047,7 @@
       <c r="A17" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B17" s="3" t="n">
+      <c r="B17" s="6" t="n">
         <v>0.93</v>
       </c>
     </row>
@@ -708,7 +1055,7 @@
       <c r="A18" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="B18" s="3" t="n">
+      <c r="B18" s="6" t="n">
         <v>0.93</v>
       </c>
     </row>
@@ -716,7 +1063,7 @@
       <c r="A19" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="B19" s="3" t="n">
+      <c r="B19" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -724,7 +1071,7 @@
       <c r="A20" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="B20" s="3" t="n">
+      <c r="B20" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -732,7 +1079,7 @@
       <c r="A21" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="B21" s="3" t="n">
+      <c r="B21" s="6" t="n">
         <v>0.93</v>
       </c>
     </row>
@@ -740,7 +1087,7 @@
       <c r="A22" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="B22" s="3" t="n">
+      <c r="B22" s="6" t="n">
         <v>0.93</v>
       </c>
     </row>
@@ -748,7 +1095,7 @@
       <c r="A23" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="B23" s="3" t="n">
+      <c r="B23" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -756,7 +1103,7 @@
       <c r="A24" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="B24" s="3" t="n">
+      <c r="B24" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -764,7 +1111,7 @@
       <c r="A25" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="B25" s="3" t="n">
+      <c r="B25" s="6" t="n">
         <v>0.93</v>
       </c>
     </row>
@@ -772,7 +1119,7 @@
       <c r="A26" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="B26" s="3" t="n">
+      <c r="B26" s="6" t="n">
         <v>0.93</v>
       </c>
     </row>
@@ -780,7 +1127,7 @@
       <c r="A27" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="B27" s="3" t="n">
+      <c r="B27" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -788,7 +1135,7 @@
       <c r="A28" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="B28" s="3" t="n">
+      <c r="B28" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -810,7 +1157,7 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -821,39 +1168,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="n">
-        <f aca="false">Rider!B4</f>
+        <f aca="false">Overview!B1</f>
         <v>299</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -861,7 +1208,7 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -869,7 +1216,7 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="5" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -877,7 +1224,7 @@
       <c r="A8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="5" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -885,7 +1232,7 @@
       <c r="A9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -893,7 +1240,7 @@
       <c r="A10" s="1" t="n">
         <v>145</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -901,7 +1248,7 @@
       <c r="A11" s="0" t="n">
         <v>145</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -909,7 +1256,7 @@
       <c r="A12" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -932,7 +1279,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -942,39 +1289,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="n">
-        <f aca="false">Rider!B4</f>
+        <f aca="false">Overview!B1</f>
         <v>299</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -982,7 +1329,7 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -990,7 +1337,7 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="5" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -998,7 +1345,7 @@
       <c r="A8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="5" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -1006,7 +1353,7 @@
       <c r="A9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -1014,7 +1361,7 @@
       <c r="A10" s="1" t="n">
         <v>235</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -1022,7 +1369,7 @@
       <c r="A11" s="0" t="n">
         <v>235</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -1030,7 +1377,7 @@
       <c r="A12" s="1" t="n">
         <v>240</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1053,7 +1400,7 @@
   <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1063,39 +1410,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="n">
-        <f aca="false">Rider!B4</f>
+        <f aca="false">Overview!B1</f>
         <v>299</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.46</v>
       </c>
     </row>
@@ -1103,7 +1450,7 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.46</v>
       </c>
     </row>
@@ -1111,7 +1458,7 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="5" t="n">
         <v>0.52</v>
       </c>
     </row>
@@ -1119,7 +1466,7 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="5" t="n">
         <v>0.52</v>
       </c>
     </row>
@@ -1127,7 +1474,7 @@
       <c r="A9" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="5" t="n">
         <v>0.58</v>
       </c>
     </row>
@@ -1135,7 +1482,7 @@
       <c r="A10" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="5" t="n">
         <v>0.58</v>
       </c>
     </row>
@@ -1143,7 +1490,7 @@
       <c r="A11" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="5" t="n">
         <v>0.64</v>
       </c>
     </row>
@@ -1151,7 +1498,7 @@
       <c r="A12" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="5" t="n">
         <v>0.64</v>
       </c>
     </row>
@@ -1159,7 +1506,7 @@
       <c r="A13" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="5" t="n">
         <v>0.7</v>
       </c>
     </row>
@@ -1167,7 +1514,7 @@
       <c r="A14" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="5" t="n">
         <v>0.7</v>
       </c>
     </row>
@@ -1175,7 +1522,7 @@
       <c r="A15" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="5" t="n">
         <v>0.76</v>
       </c>
     </row>
@@ -1183,7 +1530,7 @@
       <c r="A16" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="5" t="n">
         <v>0.76</v>
       </c>
     </row>
@@ -1191,7 +1538,7 @@
       <c r="A17" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" s="5" t="n">
         <v>0.82</v>
       </c>
     </row>
@@ -1199,7 +1546,7 @@
       <c r="A18" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" s="5" t="n">
         <v>0.82</v>
       </c>
     </row>
@@ -1207,7 +1554,7 @@
       <c r="A19" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="5" t="n">
         <v>0.88</v>
       </c>
     </row>
@@ -1215,7 +1562,7 @@
       <c r="A20" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="5" t="n">
         <v>0.88</v>
       </c>
     </row>
@@ -1223,7 +1570,7 @@
       <c r="A21" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="5" t="n">
         <v>0.94</v>
       </c>
     </row>
@@ -1231,7 +1578,7 @@
       <c r="A22" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B22" s="2" t="n">
+      <c r="B22" s="5" t="n">
         <v>0.94</v>
       </c>
     </row>
@@ -1239,7 +1586,7 @@
       <c r="A23" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B23" s="2" t="n">
+      <c r="B23" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1247,7 +1594,7 @@
       <c r="A24" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B24" s="2" t="n">
+      <c r="B24" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1255,7 +1602,7 @@
       <c r="A25" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B25" s="2" t="n">
+      <c r="B25" s="5" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -1263,7 +1610,7 @@
       <c r="A26" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B26" s="2" t="n">
+      <c r="B26" s="5" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -1271,7 +1618,7 @@
       <c r="A27" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B27" s="2" t="n">
+      <c r="B27" s="5" t="n">
         <v>1.12</v>
       </c>
     </row>
@@ -1279,7 +1626,7 @@
       <c r="A28" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B28" s="2" t="n">
+      <c r="B28" s="5" t="n">
         <v>1.12</v>
       </c>
     </row>
@@ -1287,7 +1634,7 @@
       <c r="A29" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B29" s="2" t="n">
+      <c r="B29" s="5" t="n">
         <v>1.18</v>
       </c>
     </row>
@@ -1295,7 +1642,7 @@
       <c r="A30" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B30" s="2" t="n">
+      <c r="B30" s="5" t="n">
         <v>1.18</v>
       </c>
     </row>
@@ -1303,7 +1650,7 @@
       <c r="A31" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B31" s="2" t="n">
+      <c r="B31" s="5" t="n">
         <v>1.24</v>
       </c>
     </row>
@@ -1311,7 +1658,7 @@
       <c r="A32" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B32" s="2" t="n">
+      <c r="B32" s="5" t="n">
         <v>1.24</v>
       </c>
     </row>
@@ -1319,7 +1666,7 @@
       <c r="A33" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B33" s="2" t="n">
+      <c r="B33" s="5" t="n">
         <v>1.3</v>
       </c>
     </row>
@@ -1327,7 +1674,7 @@
       <c r="A34" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B34" s="2" t="n">
+      <c r="B34" s="5" t="n">
         <v>1.3</v>
       </c>
     </row>
@@ -1335,7 +1682,7 @@
       <c r="A35" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B35" s="2" t="n">
+      <c r="B35" s="5" t="n">
         <v>1.36</v>
       </c>
     </row>
@@ -1343,7 +1690,7 @@
       <c r="A36" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B36" s="2" t="n">
+      <c r="B36" s="5" t="n">
         <v>1.36</v>
       </c>
     </row>
@@ -1351,7 +1698,7 @@
       <c r="A37" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B37" s="2" t="n">
+      <c r="B37" s="5" t="n">
         <v>1.42</v>
       </c>
     </row>
@@ -1359,7 +1706,7 @@
       <c r="A38" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B38" s="2" t="n">
+      <c r="B38" s="5" t="n">
         <v>1.42</v>
       </c>
     </row>
@@ -1367,7 +1714,7 @@
       <c r="A39" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B39" s="2" t="n">
+      <c r="B39" s="5" t="n">
         <v>1.48</v>
       </c>
     </row>
@@ -1375,7 +1722,7 @@
       <c r="A40" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B40" s="2" t="n">
+      <c r="B40" s="5" t="n">
         <v>1.48</v>
       </c>
     </row>
@@ -1383,7 +1730,7 @@
       <c r="A41" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B41" s="2" t="n">
+      <c r="B41" s="5" t="n">
         <v>1.54</v>
       </c>
     </row>
@@ -1391,7 +1738,7 @@
       <c r="A42" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B42" s="2" t="n">
+      <c r="B42" s="5" t="n">
         <v>1.54</v>
       </c>
     </row>
@@ -1399,7 +1746,7 @@
       <c r="A43" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B43" s="2" t="n">
+      <c r="B43" s="5" t="n">
         <v>1.6</v>
       </c>
     </row>
@@ -1407,7 +1754,7 @@
       <c r="A44" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B44" s="2" t="n">
+      <c r="B44" s="5" t="n">
         <v>1.6</v>
       </c>
     </row>
@@ -1415,7 +1762,7 @@
       <c r="A45" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B45" s="2" t="n">
+      <c r="B45" s="5" t="n">
         <v>1.66</v>
       </c>
     </row>
@@ -1423,7 +1770,7 @@
       <c r="A46" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B46" s="2" t="n">
+      <c r="B46" s="5" t="n">
         <v>1.66</v>
       </c>
     </row>
@@ -1431,7 +1778,7 @@
       <c r="A47" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B47" s="2" t="n">
+      <c r="B47" s="5" t="n">
         <v>0.4</v>
       </c>
     </row>
@@ -1439,7 +1786,7 @@
       <c r="A48" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B48" s="2" t="n">
+      <c r="B48" s="5" t="n">
         <v>0.3</v>
       </c>
     </row>
@@ -1461,8 +1808,8 @@
   </sheetPr>
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1472,39 +1819,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="n">
-        <f aca="false">Rider!B4</f>
+        <f aca="false">Overview!B1</f>
         <v>299</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1512,7 +1859,7 @@
       <c r="A6" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1520,7 +1867,7 @@
       <c r="A7" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="5" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -1528,7 +1875,7 @@
       <c r="A8" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="5" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -1536,7 +1883,7 @@
       <c r="A9" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1544,7 +1891,7 @@
       <c r="A10" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1552,7 +1899,7 @@
       <c r="A11" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1560,7 +1907,7 @@
       <c r="A12" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1568,7 +1915,7 @@
       <c r="A13" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="6" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -1576,7 +1923,7 @@
       <c r="A14" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="6" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -1584,7 +1931,7 @@
       <c r="A15" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1592,7 +1939,7 @@
       <c r="A16" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1600,7 +1947,7 @@
       <c r="A17" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B17" s="3" t="n">
+      <c r="B17" s="6" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -1608,7 +1955,7 @@
       <c r="A18" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B18" s="3" t="n">
+      <c r="B18" s="6" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -1616,7 +1963,7 @@
       <c r="A19" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B19" s="3" t="n">
+      <c r="B19" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1624,7 +1971,7 @@
       <c r="A20" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B20" s="3" t="n">
+      <c r="B20" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1632,7 +1979,7 @@
       <c r="A21" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B21" s="3" t="n">
+      <c r="B21" s="6" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -1640,7 +1987,7 @@
       <c r="A22" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B22" s="3" t="n">
+      <c r="B22" s="6" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -1648,7 +1995,7 @@
       <c r="A23" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B23" s="3" t="n">
+      <c r="B23" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1656,7 +2003,7 @@
       <c r="A24" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B24" s="3" t="n">
+      <c r="B24" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1664,7 +2011,7 @@
       <c r="A25" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B25" s="3" t="n">
+      <c r="B25" s="6" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -1672,7 +2019,7 @@
       <c r="A26" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B26" s="3" t="n">
+      <c r="B26" s="6" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -1680,7 +2027,7 @@
       <c r="A27" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B27" s="3" t="n">
+      <c r="B27" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1688,7 +2035,7 @@
       <c r="A28" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="B28" s="3" t="n">
+      <c r="B28" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1721,39 +2068,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="n">
-        <f aca="false">Rider!B4</f>
+        <f aca="false">Overview!B1</f>
         <v>299</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1761,7 +2108,7 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1769,7 +2116,7 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="5" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -1777,7 +2124,7 @@
       <c r="A8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="5" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -1785,7 +2132,7 @@
       <c r="A9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -1793,7 +2140,7 @@
       <c r="A10" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -1801,7 +2148,7 @@
       <c r="A11" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -1809,7 +2156,7 @@
       <c r="A12" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1842,39 +2189,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="n">
-        <f aca="false">Rider!B4</f>
+        <f aca="false">Overview!B1</f>
         <v>299</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1882,7 +2229,7 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1890,7 +2237,7 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="5" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -1898,7 +2245,7 @@
       <c r="A8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="5" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -1906,7 +2253,7 @@
       <c r="A9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -1914,7 +2261,7 @@
       <c r="A10" s="1" t="n">
         <v>115</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -1922,7 +2269,7 @@
       <c r="A11" s="0" t="n">
         <v>115</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -1930,7 +2277,7 @@
       <c r="A12" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1963,39 +2310,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="n">
-        <f aca="false">Rider!B4</f>
+        <f aca="false">Overview!B1</f>
         <v>299</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>28</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2003,7 +2350,7 @@
       <c r="A6" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2011,7 +2358,7 @@
       <c r="A7" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="5" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -2019,7 +2366,7 @@
       <c r="A8" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="5" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -2027,7 +2374,7 @@
       <c r="A9" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2035,7 +2382,7 @@
       <c r="A10" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2043,7 +2390,7 @@
       <c r="A11" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2051,7 +2398,7 @@
       <c r="A12" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2059,7 +2406,7 @@
       <c r="A13" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="6" t="n">
         <v>0.93</v>
       </c>
     </row>
@@ -2067,7 +2414,7 @@
       <c r="A14" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="6" t="n">
         <v>0.93</v>
       </c>
     </row>
@@ -2075,7 +2422,7 @@
       <c r="A15" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2083,7 +2430,7 @@
       <c r="A16" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2091,7 +2438,7 @@
       <c r="A17" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B17" s="3" t="n">
+      <c r="B17" s="6" t="n">
         <v>0.93</v>
       </c>
     </row>
@@ -2099,7 +2446,7 @@
       <c r="A18" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B18" s="3" t="n">
+      <c r="B18" s="6" t="n">
         <v>0.93</v>
       </c>
     </row>
@@ -2107,7 +2454,7 @@
       <c r="A19" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B19" s="3" t="n">
+      <c r="B19" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2115,7 +2462,7 @@
       <c r="A20" s="0" t="n">
         <v>54</v>
       </c>
-      <c r="B20" s="3" t="n">
+      <c r="B20" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2123,7 +2470,7 @@
       <c r="A21" s="0" t="n">
         <v>54</v>
       </c>
-      <c r="B21" s="3" t="n">
+      <c r="B21" s="6" t="n">
         <v>0.93</v>
       </c>
     </row>
@@ -2131,7 +2478,7 @@
       <c r="A22" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="B22" s="3" t="n">
+      <c r="B22" s="6" t="n">
         <v>0.93</v>
       </c>
     </row>
@@ -2139,7 +2486,7 @@
       <c r="A23" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="B23" s="3" t="n">
+      <c r="B23" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2147,7 +2494,7 @@
       <c r="A24" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="B24" s="3" t="n">
+      <c r="B24" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2155,7 +2502,7 @@
       <c r="A25" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="B25" s="3" t="n">
+      <c r="B25" s="6" t="n">
         <v>0.93</v>
       </c>
     </row>
@@ -2163,7 +2510,7 @@
       <c r="A26" s="0" t="n">
         <v>83</v>
       </c>
-      <c r="B26" s="3" t="n">
+      <c r="B26" s="6" t="n">
         <v>0.93</v>
       </c>
     </row>
@@ -2171,7 +2518,7 @@
       <c r="A27" s="0" t="n">
         <v>83</v>
       </c>
-      <c r="B27" s="3" t="n">
+      <c r="B27" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2179,7 +2526,7 @@
       <c r="A28" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="B28" s="3" t="n">
+      <c r="B28" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2212,39 +2559,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="n">
-        <f aca="false">Rider!B4</f>
+        <f aca="false">Overview!B1</f>
         <v>299</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2252,7 +2599,7 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2260,7 +2607,7 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="5" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -2268,7 +2615,7 @@
       <c r="A8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="5" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -2276,7 +2623,7 @@
       <c r="A9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -2284,7 +2631,7 @@
       <c r="A10" s="1" t="n">
         <v>145</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -2292,7 +2639,7 @@
       <c r="A11" s="0" t="n">
         <v>145</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -2300,7 +2647,7 @@
       <c r="A12" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2333,39 +2680,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="n">
-        <f aca="false">Rider!B4</f>
+        <f aca="false">Overview!B1</f>
         <v>299</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2373,7 +2720,7 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2381,7 +2728,7 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="5" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -2389,7 +2736,7 @@
       <c r="A8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="5" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -2397,7 +2744,7 @@
       <c r="A9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -2405,7 +2752,7 @@
       <c r="A10" s="1" t="n">
         <v>235</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -2413,7 +2760,7 @@
       <c r="A11" s="0" t="n">
         <v>235</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="5" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -2421,7 +2768,7 @@
       <c r="A12" s="1" t="n">
         <v>240</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2454,39 +2801,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="n">
-        <f aca="false">Rider!B4</f>
+        <f aca="false">Overview!B1</f>
         <v>299</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2494,7 +2841,7 @@
       <c r="A6" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2502,7 +2849,7 @@
       <c r="A7" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="5" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -2510,7 +2857,7 @@
       <c r="A8" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="5" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -2518,7 +2865,7 @@
       <c r="A9" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2526,7 +2873,7 @@
       <c r="A10" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2534,7 +2881,7 @@
       <c r="A11" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2542,7 +2889,7 @@
       <c r="A12" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="5" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2550,7 +2897,7 @@
       <c r="A13" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="6" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -2558,7 +2905,7 @@
       <c r="A14" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="6" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -2566,7 +2913,7 @@
       <c r="A15" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2574,7 +2921,7 @@
       <c r="A16" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2582,7 +2929,7 @@
       <c r="A17" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B17" s="3" t="n">
+      <c r="B17" s="6" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -2590,7 +2937,7 @@
       <c r="A18" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B18" s="3" t="n">
+      <c r="B18" s="6" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -2598,7 +2945,7 @@
       <c r="A19" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B19" s="3" t="n">
+      <c r="B19" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2606,7 +2953,7 @@
       <c r="A20" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B20" s="3" t="n">
+      <c r="B20" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2614,7 +2961,7 @@
       <c r="A21" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B21" s="3" t="n">
+      <c r="B21" s="6" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -2622,7 +2969,7 @@
       <c r="A22" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B22" s="3" t="n">
+      <c r="B22" s="6" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -2630,7 +2977,7 @@
       <c r="A23" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B23" s="3" t="n">
+      <c r="B23" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2638,7 +2985,7 @@
       <c r="A24" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="B24" s="3" t="n">
+      <c r="B24" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2646,7 +2993,7 @@
       <c r="A25" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="B25" s="3" t="n">
+      <c r="B25" s="6" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -2654,7 +3001,7 @@
       <c r="A26" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="B26" s="3" t="n">
+      <c r="B26" s="6" t="n">
         <v>1.06</v>
       </c>
     </row>
@@ -2662,7 +3009,7 @@
       <c r="A27" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="B27" s="3" t="n">
+      <c r="B27" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2670,7 +3017,7 @@
       <c r="A28" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="B28" s="3" t="n">
+      <c r="B28" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>